<commit_message>
started estimating tpr in target pop
</commit_message>
<xml_diff>
--- a/data/target_pop_data.xlsx
+++ b/data/target_pop_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julietfleischer/Documents/NYPD_SQF_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D764F-1E30-6348-A8AC-A70B0A770D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BDF458-7FDE-A447-B3E8-5F1779C8ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16840" activeTab="4" xr2:uid="{21416674-CDA2-AF4F-9A4C-5CB761AD2769}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Manhatten" sheetId="5" r:id="rId2"/>
     <sheet name="Bronx" sheetId="6" r:id="rId3"/>
     <sheet name="Queens" sheetId="4" r:id="rId4"/>
-    <sheet name="Staten_Island" sheetId="3" r:id="rId5"/>
+    <sheet name="Staten Island" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
added information and graphics about general crime rates
</commit_message>
<xml_diff>
--- a/data/target_pop_data.xlsx
+++ b/data/target_pop_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julietfleischer/Documents/NYPD_SQF_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BDF458-7FDE-A447-B3E8-5F1779C8ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E4A7D-2C34-B146-A1DD-938A42ECE6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16840" activeTab="4" xr2:uid="{21416674-CDA2-AF4F-9A4C-5CB761AD2769}"/>
+    <workbookView xWindow="6120" yWindow="22520" windowWidth="28240" windowHeight="16840" activeTab="4" xr2:uid="{21416674-CDA2-AF4F-9A4C-5CB761AD2769}"/>
   </bookViews>
   <sheets>
     <sheet name="Brooklyn" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="98">
   <si>
     <t>Number</t>
   </si>
@@ -143,9 +143,6 @@
     <t>-1.1</t>
   </si>
   <si>
-    <t>2,736,074</t>
-  </si>
-  <si>
     <t>-6,068,116</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>0.7</t>
   </si>
   <si>
-    <t>2,405,464</t>
-  </si>
-  <si>
     <t>-6,398,726</t>
   </si>
   <si>
@@ -236,9 +230,6 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>1,694,251</t>
-  </si>
-  <si>
     <t>-7,109,939</t>
   </si>
   <si>
@@ -285,9 +276,6 @@
   </si>
   <si>
     <t>0.3</t>
-  </si>
-  <si>
-    <t>1,472,654</t>
   </si>
   <si>
     <t>-7,331,536</t>
@@ -336,6 +324,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -776,7 +767,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -819,13 +810,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -856,6 +852,7 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="42" builtinId="3"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1202,16 +1199,19 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" style="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1231,8 +1231,8 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>39</v>
+      <c r="B2" s="3">
+        <v>2736074</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1244,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1254,11 +1254,11 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1">
-        <v>516.42600000000004</v>
+      <c r="B3" s="3">
+        <v>516426</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -1267,21 +1267,21 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
         <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1">
-        <v>968.42700000000002</v>
+      <c r="B4" s="3">
+        <v>968427</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -1290,7 +1290,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2">
         <v>45781</v>
@@ -1300,11 +1300,11 @@
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1">
-        <v>729.69600000000003</v>
+      <c r="B5" s="3">
+        <v>729696</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>21</v>
@@ -1313,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2">
         <v>45783</v>
@@ -1323,11 +1323,11 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="1">
-        <v>370.77600000000001</v>
+      <c r="B6" s="3">
+        <v>370776</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>27</v>
@@ -1336,21 +1336,21 @@
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
         <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1">
-        <v>37.579000000000001</v>
+      <c r="B7" s="3">
+        <v>37579</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1">
         <v>143.63200000000001</v>
@@ -1362,18 +1362,18 @@
         <v>-106.053</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1">
-        <v>113.17</v>
+      <c r="B8" s="3">
+        <v>113170</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1">
         <v>299.959</v>
@@ -1385,12 +1385,12 @@
         <v>-186.78899999999999</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1398,7 +1398,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1406,7 +1406,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1421,17 +1421,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C22D75-4B2B-7C4F-884C-38B93453E85B}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1451,8 +1454,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>70</v>
+      <c r="B2" s="5">
+        <v>1694251</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1464,7 +1467,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1474,11 +1477,11 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>402.64</v>
+      <c r="B3" s="5">
+        <v>402640</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1487,21 +1490,21 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>793.29399999999998</v>
+      <c r="B4" s="5">
+        <v>793294</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1510,7 +1513,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G4" s="2">
         <v>45915</v>
@@ -1520,11 +1523,11 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
-        <v>199.59200000000001</v>
+      <c r="B5" s="5">
+        <v>199592</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1533,21 +1536,21 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
-        <v>219.624</v>
+      <c r="B6" s="5">
+        <v>219624</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1556,21 +1559,21 @@
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>16.111999999999998</v>
+      <c r="B7" s="5">
+        <v>16112</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D7">
         <v>143.63200000000001</v>
@@ -1582,18 +1585,18 @@
         <v>-127.52</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>62.988999999999997</v>
+      <c r="B8" s="5">
+        <v>62989</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>299.959</v>
@@ -1605,7 +1608,7 @@
         <v>-236.97</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1617,17 +1620,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5B9137-9942-0943-A3C8-769C18D5877E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="210" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1647,8 +1653,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>87</v>
+      <c r="B2" s="5">
+        <v>1472654</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1660,7 +1666,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1670,11 +1676,11 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>806.46299999999997</v>
+      <c r="B3" s="5">
+        <v>806463</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1683,7 +1689,7 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G3" s="2">
         <v>45803</v>
@@ -1693,11 +1699,11 @@
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>130.79599999999999</v>
+      <c r="B4" s="5">
+        <v>130796</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1706,21 +1712,21 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
-        <v>419.39299999999997</v>
+      <c r="B5" s="5">
+        <v>419393</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1729,7 +1735,7 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G5" s="2">
         <v>45724</v>
@@ -1739,11 +1745,11 @@
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
-        <v>67.766000000000005</v>
+      <c r="B6" s="5">
+        <v>67766</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1752,21 +1758,21 @@
         <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>19.866</v>
+      <c r="B7" s="5">
+        <v>19866</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <v>143.63200000000001</v>
@@ -1778,18 +1784,18 @@
         <v>-123.76600000000001</v>
       </c>
       <c r="G7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>28.37</v>
+      <c r="B8" s="5">
+        <v>28370</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D8">
         <v>299.959</v>
@@ -1801,7 +1807,7 @@
         <v>-271.589</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1813,17 +1819,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A3BD87-1455-E243-AA4F-CA9E9542653F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="167" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1843,8 +1852,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
+      <c r="B2" s="6">
+        <v>2405464</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1856,7 +1865,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1866,11 +1875,11 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>667.86099999999999</v>
+      <c r="B3" s="5">
+        <v>667861</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1879,21 +1888,21 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>549.35799999999995</v>
+      <c r="B4" s="5">
+        <v>549358</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -1902,21 +1911,21 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
-        <v>381.375</v>
+      <c r="B5" s="5">
+        <v>381375</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -1925,21 +1934,21 @@
         <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6">
-        <v>656.58299999999997</v>
+      <c r="B6" s="5">
+        <v>656583</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1958,11 +1967,11 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>66.174999999999997</v>
+      <c r="B7" s="5">
+        <v>66175</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>143.63200000000001</v>
@@ -1981,11 +1990,11 @@
       <c r="A8" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>84.111999999999995</v>
+      <c r="B8" s="5">
+        <v>84112</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>299.959</v>
@@ -1997,7 +2006,7 @@
         <v>-215.84700000000001</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2009,8 +2018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF7A6C1-1CE4-2840-8385-CE64A2230BAD}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2040,7 +2049,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>495.74700000000001</v>
+        <v>495747</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2063,7 +2072,7 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>96.96</v>
+        <v>96960</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -2086,7 +2095,7 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>277.98099999999999</v>
+        <v>277981</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -2109,7 +2118,7 @@
         <v>19</v>
       </c>
       <c r="B5">
-        <v>46.835000000000001</v>
+        <v>46835</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -2132,7 +2141,7 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>58.753</v>
+        <v>58753</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -2155,7 +2164,7 @@
         <v>31</v>
       </c>
       <c r="B7">
-        <v>3.9</v>
+        <v>3900</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -2178,7 +2187,7 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>11.318</v>
+        <v>11318</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>

</xml_diff>